<commit_message>
change on card: adding photo placeholder
</commit_message>
<xml_diff>
--- a/colaboradores.xlsx
+++ b/colaboradores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanlozanovargas/dev/suraelec-cards/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanjose/webDev/suraelec/sura-cards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FB9097-878B-0744-A28E-E15E48E41252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A659C5E-7F07-3149-8674-199BF953CAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{430F15BD-6BF9-D14C-B148-D5B4474620E2}"/>
+    <workbookView xWindow="1360" yWindow="740" windowWidth="28040" windowHeight="17140" xr2:uid="{430F15BD-6BF9-D14C-B148-D5B4474620E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>id</t>
   </si>
@@ -53,47 +53,32 @@
     <t>email</t>
   </si>
   <si>
-    <t>Juanito Prueba</t>
-  </si>
-  <si>
-    <t>Juanito Test</t>
-  </si>
-  <si>
-    <t>Juanito Max</t>
-  </si>
-  <si>
-    <t>Juanito Ultra</t>
-  </si>
-  <si>
-    <t>Gerente</t>
-  </si>
-  <si>
-    <t>Gerente de gerencia</t>
-  </si>
-  <si>
-    <t>Gerente general</t>
-  </si>
-  <si>
-    <t>Supergerente</t>
-  </si>
-  <si>
-    <t>Tets@uno.com</t>
-  </si>
-  <si>
     <t>Tets@dps.com</t>
   </si>
   <si>
     <t>Tets@tres.com</t>
   </si>
   <si>
-    <t>Tets@cuatro.com</t>
+    <t>Anyerson Buitrago</t>
+  </si>
+  <si>
+    <t>Comercial</t>
+  </si>
+  <si>
+    <t>William Romero</t>
+  </si>
+  <si>
+    <t>Andrea Manzi</t>
+  </si>
+  <si>
+    <t>pendiente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -105,13 +90,6 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -140,8 +118,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -161,8 +139,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9C7E308C-F933-7346-A8E7-B89CE627F072}" name="Table1" displayName="Table1" ref="A1:E5" totalsRowShown="0">
-  <autoFilter ref="A1:E5" xr:uid="{9C7E308C-F933-7346-A8E7-B89CE627F072}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9C7E308C-F933-7346-A8E7-B89CE627F072}" name="Table1" displayName="Table1" ref="A1:E4" totalsRowShown="0">
+  <autoFilter ref="A1:E4" xr:uid="{9C7E308C-F933-7346-A8E7-B89CE627F072}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{3802CE75-12EA-D244-8680-7D04113C2AA3}" name="id"/>
     <tableColumn id="2" xr3:uid="{84A8A950-7E7B-6649-BFBB-27AA50BC3CB3}" name="name"/>
@@ -491,15 +469,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A78D11E8-15F9-2F47-BA40-24B5E4FE74EE}">
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:E1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -524,16 +503,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2">
+        <v>573187079284</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2">
-        <v>3505121212</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -541,16 +520,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2">
+        <v>573168315138</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>3505121213</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -558,48 +537,30 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1">
-        <v>3505121215</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>15</v>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>3505121216</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="1048576" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1048576" s="2"/>
+    <row r="1048575" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E1048575" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{178F0FE8-60D8-C844-822A-C508F57E6246}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{BCFB9B38-465A-934D-9028-AED201F5C58D}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{AE2AAE89-8CF5-B046-8AF3-710EA7E9826A}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{EED6927B-C52C-FB41-A2C7-4948FB891DAE}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{BCFB9B38-465A-934D-9028-AED201F5C58D}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{AE2AAE89-8CF5-B046-8AF3-710EA7E9826A}"/>
+    <hyperlink ref="E4" r:id="rId3" display="Tets@cuatro.com" xr:uid="{EED6927B-C52C-FB41-A2C7-4948FB891DAE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update collaborator data handling and templates: added 'profile' field to Excel import, modified HTML templates for displaying collaborator information, and removed unnecessary files.
</commit_message>
<xml_diff>
--- a/colaboradores.xlsx
+++ b/colaboradores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanjose/webDev/suraelec/sura-cards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A659C5E-7F07-3149-8674-199BF953CAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30875A09-C3DE-5C44-842B-B3A42B7E7D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="740" windowWidth="28040" windowHeight="17140" xr2:uid="{430F15BD-6BF9-D14C-B148-D5B4474620E2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>id</t>
   </si>
@@ -53,12 +53,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>Tets@dps.com</t>
-  </si>
-  <si>
-    <t>Tets@tres.com</t>
-  </si>
-  <si>
     <t>Anyerson Buitrago</t>
   </si>
   <si>
@@ -72,6 +66,18 @@
   </si>
   <si>
     <t>pendiente</t>
+  </si>
+  <si>
+    <t>profile</t>
+  </si>
+  <si>
+    <t>wromero@suraelec.com</t>
+  </si>
+  <si>
+    <t>abuitrago@suraelec.com</t>
+  </si>
+  <si>
+    <t>amanzi@suraelec.com</t>
   </si>
 </sst>
 </file>
@@ -139,14 +145,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9C7E308C-F933-7346-A8E7-B89CE627F072}" name="Table1" displayName="Table1" ref="A1:E4" totalsRowShown="0">
-  <autoFilter ref="A1:E4" xr:uid="{9C7E308C-F933-7346-A8E7-B89CE627F072}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9C7E308C-F933-7346-A8E7-B89CE627F072}" name="Table1" displayName="Table1" ref="A1:F4" totalsRowShown="0">
+  <autoFilter ref="A1:F4" xr:uid="{9C7E308C-F933-7346-A8E7-B89CE627F072}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{3802CE75-12EA-D244-8680-7D04113C2AA3}" name="id"/>
     <tableColumn id="2" xr3:uid="{84A8A950-7E7B-6649-BFBB-27AA50BC3CB3}" name="name"/>
     <tableColumn id="3" xr3:uid="{B8BBBD78-585F-734E-B96C-5AFB3A3DCC05}" name="position"/>
     <tableColumn id="4" xr3:uid="{7C90B699-FE23-8346-B1A7-BDFEE568BB51}" name="phone"/>
     <tableColumn id="5" xr3:uid="{BFBD1AFA-56F3-8B43-AF09-EBD42CB80D50}" name="email" dataCellStyle="Hyperlink"/>
+    <tableColumn id="6" xr3:uid="{D220C466-96F4-E249-9A04-F924B4923D77}" name="profile"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -469,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A78D11E8-15F9-2F47-BA40-24B5E4FE74EE}">
-  <dimension ref="A1:E1048575"/>
+  <dimension ref="A1:F1048574"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -481,7 +488,7 @@
     <col min="4" max="4" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -497,66 +504,69 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2">
         <v>573187079284</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3" s="2">
         <v>573168315138</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="1048575" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1048575" s="1"/>
+    <row r="1048574" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E1048574" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{BCFB9B38-465A-934D-9028-AED201F5C58D}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{AE2AAE89-8CF5-B046-8AF3-710EA7E9826A}"/>
-    <hyperlink ref="E4" r:id="rId3" display="Tets@cuatro.com" xr:uid="{EED6927B-C52C-FB41-A2C7-4948FB891DAE}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{EED6927B-C52C-FB41-A2C7-4948FB891DAE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
change on card: last change
</commit_message>
<xml_diff>
--- a/colaboradores.xlsx
+++ b/colaboradores.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanjose/webDev/suraelec/sura-cards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30875A09-C3DE-5C44-842B-B3A42B7E7D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD0E4D8-4FD7-F544-9E9F-0F552B37594A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="740" windowWidth="28040" windowHeight="17140" xr2:uid="{430F15BD-6BF9-D14C-B148-D5B4474620E2}"/>
+    <workbookView xWindow="1360" yWindow="680" windowWidth="28040" windowHeight="17140" xr2:uid="{430F15BD-6BF9-D14C-B148-D5B4474620E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>id</t>
   </si>
@@ -78,6 +78,30 @@
   </si>
   <si>
     <t>amanzi@suraelec.com</t>
+  </si>
+  <si>
+    <t>Ricardo Avila</t>
+  </si>
+  <si>
+    <t>ravila@suraelec.com</t>
+  </si>
+  <si>
+    <t>Celina Charris</t>
+  </si>
+  <si>
+    <t>Lider Regional</t>
+  </si>
+  <si>
+    <t>ccharris@suraelec.com</t>
+  </si>
+  <si>
+    <t>Juan J Lozano</t>
+  </si>
+  <si>
+    <t>Gerente</t>
+  </si>
+  <si>
+    <t>jlozano@suraelec.com</t>
   </si>
 </sst>
 </file>
@@ -145,8 +169,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9C7E308C-F933-7346-A8E7-B89CE627F072}" name="Table1" displayName="Table1" ref="A1:F4" totalsRowShown="0">
-  <autoFilter ref="A1:F4" xr:uid="{9C7E308C-F933-7346-A8E7-B89CE627F072}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9C7E308C-F933-7346-A8E7-B89CE627F072}" name="Table1" displayName="Table1" ref="A1:F7" totalsRowShown="0">
+  <autoFilter ref="A1:F7" xr:uid="{9C7E308C-F933-7346-A8E7-B89CE627F072}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{3802CE75-12EA-D244-8680-7D04113C2AA3}" name="id"/>
     <tableColumn id="2" xr3:uid="{84A8A950-7E7B-6649-BFBB-27AA50BC3CB3}" name="name"/>
@@ -479,13 +503,15 @@
   <dimension ref="A1:F1048574"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -559,6 +585,57 @@
         <v>13</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2">
+        <v>573163215029</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2">
+        <v>573183117195</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2">
+        <v>573164763846</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="1048574" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E1048574" s="1"/>
     </row>
@@ -567,10 +644,13 @@
     <hyperlink ref="E2" r:id="rId1" xr:uid="{BCFB9B38-465A-934D-9028-AED201F5C58D}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{AE2AAE89-8CF5-B046-8AF3-710EA7E9826A}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{EED6927B-C52C-FB41-A2C7-4948FB891DAE}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{9D511104-34B4-084E-8BC4-F744E4C4AD54}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{FCFA8025-01C0-1340-A49A-A072FD22BAD6}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{E72B0B7F-C19E-FD4B-9025-A05966DA01D6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>